<commit_message>
post exchange rates on facebook
</commit_message>
<xml_diff>
--- a/Com.EzTender.WebApp/wwwroot/Template/RFQ_Template.xlsx
+++ b/Com.EzTender.WebApp/wwwroot/Template/RFQ_Template.xlsx
@@ -1,24 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EzyTender\Com.EzTender.WebApp\wwwroot\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EzyTender\Com.EzTender.WebApp\wwwroot\Upload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3B5560-D30F-4582-ADF8-DB63BB2DBC22}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{18F722F0-F366-4918-910F-042B7D472CEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="sla" sheetId="2" r:id="rId2"/>
-    <sheet name="penalty" sheetId="3" r:id="rId3"/>
-    <sheet name="pricing" sheetId="4" r:id="rId4"/>
+    <sheet name="supports" sheetId="2" r:id="rId2"/>
+    <sheet name="commercials" sheetId="3" r:id="rId3"/>
+    <sheet name="product pricing" sheetId="4" r:id="rId4"/>
+    <sheet name="service pricing" sheetId="5" r:id="rId5"/>
+    <sheet name="warranty pricing" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
   <si>
     <t>ServiceName</t>
   </si>
@@ -36,16 +38,13 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Reqiorement</t>
-  </si>
-  <si>
-    <t>Breach of Service Definition</t>
-  </si>
-  <si>
-    <t>Milestone</t>
-  </si>
-  <si>
-    <t>Commercial term and description</t>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service Name </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description </t>
   </si>
   <si>
     <t xml:space="preserve">Item Name </t>
@@ -101,10 +100,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -495,7 +497,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B3"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +526,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B4"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,13 +554,13 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="1025" width="8.5546875" customWidth="1"/>
   </cols>
@@ -570,9 +572,7 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="C1" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -584,13 +584,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875"/>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" customWidth="1"/>
@@ -598,27 +598,109 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="21.77734375" customWidth="1"/>
+    <col min="4" max="4" width="14.21875" customWidth="1"/>
+    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add industry certification column in company table
</commit_message>
<xml_diff>
--- a/Com.EzTender.WebApp/wwwroot/Template/RFQ_Template.xlsx
+++ b/Com.EzTender.WebApp/wwwroot/Template/RFQ_Template.xlsx
@@ -5,23 +5,27 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EzyTender\Com.EzTender.WebApp\wwwroot\Upload\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\EzyTender\Com.EzTender.WebApp\wwwroot\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{18F722F0-F366-4918-910F-042B7D472CEE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1890FF49-38CA-4F9C-826A-C1BFF1A555CC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="requirements" sheetId="1" r:id="rId1"/>
-    <sheet name="supports" sheetId="2" r:id="rId2"/>
-    <sheet name="commercials" sheetId="3" r:id="rId3"/>
-    <sheet name="product pricing" sheetId="4" r:id="rId4"/>
-    <sheet name="service pricing" sheetId="5" r:id="rId5"/>
-    <sheet name="warranty pricing" sheetId="6" r:id="rId6"/>
+    <sheet name="Product Req" sheetId="1" r:id="rId1"/>
+    <sheet name="Support Req" sheetId="2" r:id="rId2"/>
+    <sheet name="Commercial Req" sheetId="3" r:id="rId3"/>
+    <sheet name="Pricing Format" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
@@ -30,33 +34,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="9">
-  <si>
-    <t>ServiceName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Requirement</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Service Name </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description </t>
-  </si>
-  <si>
     <t xml:space="preserve">Item Name </t>
   </si>
   <si>
     <t xml:space="preserve">Item Description </t>
   </si>
   <si>
-    <t xml:space="preserve">Internal Reference Code </t>
-  </si>
-  <si>
     <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t>Warranty</t>
+  </si>
+  <si>
+    <t>Delay in Performance</t>
+  </si>
+  <si>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Warranty Period</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>1-Year</t>
+  </si>
+  <si>
+    <t>12 months warranty on products and installed services</t>
+  </si>
+  <si>
+    <t>Eg. Printer</t>
+  </si>
+  <si>
+    <t>Eg. Installation</t>
+  </si>
+  <si>
+    <t>Onsite installation</t>
+  </si>
+  <si>
+    <t>Colour Laser Printer</t>
+  </si>
+  <si>
+    <t>Support Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If there is delay in the performance of the Services or the supply of Goods due to any acts of God, force majeure, riots and civil commotion, strikes, lock-outs or other causes or perils beyond the Supplier's control, then in any such case the Supplier shall, for the duration of any such circumstances, be relieved of the obligation to perform the Services or supply the Goods thereby affected. Any part of the Services or Goods that are not so affected shall continue to be performed in accordance with the Agreement. If the Supplier fails to complete the performance of Services or supply of Goods by the date(s) specified in the Agreement, The Buyer shall have the right - (a) to cancel all or any part of such Services or Goods from the Agreement without compensation to the Supplier and to obtain the same (including similar or equivalent goods and services in the case where the exact goods and services are not available) from other sources and all increased costs incurred shall be deducted from any moneys due or to become due to the Supplier or shall be recoverable as damages; or (b) to deduct any moneys due or to become due to the Supplier or require the Supplier to pay a sum calculated at the rate of 0.5% of the Contract Price for each day of delay (including Sundays and Public Holidays), as liquidated damages until the delayed Services or Goods are fully performed or supplied; up to a maximum amount of liquidated damages equivalent to 20% of the Contract Price. This maximum amount is based on the aggregate of all liquidated damages imposed for all cases of delay during the entire period of the Agreement and is not the maximum sum for each individual case of delay. </t>
+  </si>
+  <si>
+    <t>All Services or the supply of Goods shall extend for a period of twelve (12) months following the beginning of Commercial Operation (the Warranty Period). The warranty period with respect to any Services or the supply of Goods that is repaired, replaced, modified or otherwise altered or corrected after Commercial Operation shall extend for twelve (12) months from the date of completion of such repair, replacement, modification, correction or alteration, provided that in no event shall the warranty period extend beyond twenty four (24) months from Commercial Operation.</t>
+  </si>
+  <si>
+    <t>In addition to the Supplier's warranty obligations, Supplier will provide at the Buyer's requests, reasonable service and support related to any nonconformity or defect or damage of the Services or the supply of Goods provided hereunder to the Buyer.</t>
+  </si>
+  <si>
+    <t>Colour Laser Printer:
+• High-performance – print speed up to 17 A4 pages per minute in colour, 30 ppm in monochrome
+• High-capacity toner cartridges permit optimum cost-per-page
+• Wide range of supported media including labels, envelopes, cardstock and transparencies
+• Wide range of optional accessories to maximise printer productivity
+• Easy to use graphical LCD front panel
+• Robust 60,000 pages per month duty cycle</t>
+  </si>
+  <si>
+    <t>Eg. Onsite Installation</t>
+  </si>
+  <si>
+    <t>Installation services to be provided by qualified personnel onsite.</t>
   </si>
 </sst>
 </file>
@@ -73,22 +128,33 @@
     </font>
     <font>
       <b/>
-      <sz val="7"/>
-      <color rgb="FF555555"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -96,21 +162,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,213 +600,479 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="77.77734375" style="2" customWidth="1"/>
+    <col min="4" max="1026" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1027" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="aB+tihYodDvoXanTsw001LrM47T2UQEODprQ1E/SY5rMmO6YM5TT+wItwQ9NE5+J0BT0X8w/hFFeiuXpk7NN2Q==" saltValue="P/GogIiiQJbcUbkXRYaW7Q==" spinCount="100000" sheet="1" objects="1" scenarios="1" insertRows="0" insertHyperlinks="0" deleteRows="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="77.77734375" style="2" customWidth="1"/>
+    <col min="4" max="1026" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1027" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="76GqC+Kc2sG6E/wxKc3Y+sLBl9PrZWg3iC4CGR4l26B28V0s7HLuI//7A7omOQnKPcLunj+lx9HswYHwzU9/OA==" saltValue="Li6REv2Yz5fITiV6+o/N+w==" spinCount="100000" sheet="1" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.77734375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="77.77734375" style="2" customWidth="1"/>
+    <col min="4" max="1025" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1026" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="273.60000000000002" x14ac:dyDescent="0.3">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="Id//fYZ6P5up8CgLyMYfaoEMwC7/PCRihm4YWP5J9/iWdB5hTtIc62YfF0SfJXpfLZPX0jKFyuwg7J1na60ySw==" saltValue="Fzng4g/zQ2hJpijNZ0WpVQ==" spinCount="100000" sheet="1" insertRows="0" insertHyperlinks="0" deleteRows="0" sort="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" customWidth="1"/>
-    <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="23.21875" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="32.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="4" customWidth="1"/>
+    <col min="5" max="1024" width="8.5546875" style="1" customWidth="1"/>
+    <col min="1025" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="6">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="6">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="6">
+        <v>3</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>1</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="6">
+        <v>2</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="6">
+        <v>1</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="6">
+        <v>2</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="10"/>
     </row>
   </sheetData>
+  <sheetProtection insertRows="0" deleteRows="0"/>
+  <mergeCells count="3">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A13:D13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.44140625" customWidth="1"/>
-    <col min="3" max="3" width="21.21875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.21875" customWidth="1"/>
-    <col min="5" max="1025" width="8.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>